<commit_message>
Final save 23.05.19 15:45
</commit_message>
<xml_diff>
--- a/docs/analysis/Planification.xlsx
+++ b/docs/analysis/Planification.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11880"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11880" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionnel" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="69">
   <si>
     <t>Temps nécessaire</t>
   </si>
@@ -216,6 +216,18 @@
   </si>
   <si>
     <t>Inscription Courts</t>
+  </si>
+  <si>
+    <t>Classe Esession</t>
+  </si>
+  <si>
+    <t>Utilisateurs (cours inscrit + nombre inscrpition possible)</t>
+  </si>
+  <si>
+    <t>Envoi emails</t>
+  </si>
+  <si>
+    <t>Ajax</t>
   </si>
 </sst>
 </file>
@@ -269,7 +281,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -394,11 +406,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -482,11 +518,46 @@
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="46">
+  <dxfs count="48">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1131,7 +1202,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
@@ -2293,98 +2364,98 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:M2 F38:F40 H38:I40 L3:L42 I3:I42 G3:G42 E3:E42 C3:C42">
-    <cfRule type="cellIs" dxfId="45" priority="48" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="47" priority="48" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:M2 C42:M42 C41 E41:M41 C4:M19 C21:M40">
-    <cfRule type="cellIs" dxfId="44" priority="47" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="46" priority="47" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L35 I35 G35 E35 C35">
-    <cfRule type="cellIs" dxfId="43" priority="46" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="46" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:M35">
-    <cfRule type="cellIs" dxfId="42" priority="45" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="44" priority="45" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J41:K41 F41 H41 M41">
-    <cfRule type="cellIs" dxfId="41" priority="44" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="44" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D38:D40 G38:G40 J38:K40">
-    <cfRule type="cellIs" dxfId="40" priority="43" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="43" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42:M42 C41 E41:M41 C2:M40">
-    <cfRule type="cellIs" dxfId="39" priority="40" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="40" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="41" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="40" priority="41" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="42" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="42" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N42">
-    <cfRule type="cellIs" dxfId="36" priority="33" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="38" priority="33" operator="greaterThan">
       <formula>$B2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="39" operator="equal">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43">
-    <cfRule type="cellIs" dxfId="34" priority="35" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="35" operator="greaterThan">
       <formula>3.66666666666667</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="37" operator="equal">
       <formula>3.66666666666667</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43:M43">
-    <cfRule type="cellIs" dxfId="32" priority="34" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="34" operator="greaterThan">
       <formula>0.333333333333333</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="36" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D41">
-    <cfRule type="cellIs" dxfId="30" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="32" priority="23" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D41">
-    <cfRule type="cellIs" dxfId="29" priority="22" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="22" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D41">
-    <cfRule type="cellIs" dxfId="28" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="19" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="20" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="21" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L36 I36 G36 E36 C36">
-    <cfRule type="cellIs" dxfId="25" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="11" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36:M36">
-    <cfRule type="cellIs" dxfId="24" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2542,23 +2613,23 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:D1 C2:C12">
-    <cfRule type="cellIs" dxfId="23" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="5" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:D1 C3:D10 C12:D12">
-    <cfRule type="cellIs" dxfId="22" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:D12">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2568,10 +2639,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N46"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M42" sqref="M42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2588,10 +2659,10 @@
       <c r="B1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="43" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="10" t="s">
@@ -2645,7 +2716,7 @@
       <c r="L2" s="8"/>
       <c r="M2" s="9"/>
       <c r="N2" s="3">
-        <f t="shared" ref="N2:N14" si="0">SUM(E2:M2)</f>
+        <f t="shared" ref="N2:N15" si="0">SUM(E2:M2)</f>
         <v>0</v>
       </c>
     </row>
@@ -2711,7 +2782,9 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="E5" s="4"/>
-      <c r="F5" s="12"/>
+      <c r="F5" s="12">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="G5" s="4"/>
       <c r="H5" s="12"/>
       <c r="I5" s="4"/>
@@ -2721,7 +2794,7 @@
       <c r="M5" s="13"/>
       <c r="N5" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -2772,42 +2845,39 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="18"/>
+      <c r="A8" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="18">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D8" s="42"/>
       <c r="E8" s="4"/>
       <c r="F8" s="12"/>
       <c r="G8" s="4"/>
       <c r="H8" s="12"/>
       <c r="I8" s="4"/>
-      <c r="J8" s="12"/>
+      <c r="J8" s="12">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="K8" s="12"/>
       <c r="L8" s="4"/>
       <c r="M8" s="13"/>
-      <c r="N8" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="N8" s="3"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="18">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="C9" s="42">
-        <v>0.125</v>
-      </c>
-      <c r="E9" s="1"/>
+      <c r="A9" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="18"/>
+      <c r="E9" s="4"/>
       <c r="F9" s="12"/>
-      <c r="G9" s="1"/>
+      <c r="G9" s="4"/>
       <c r="H9" s="12"/>
-      <c r="I9" s="1"/>
+      <c r="I9" s="4"/>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
-      <c r="L9" s="1"/>
+      <c r="L9" s="4"/>
       <c r="M9" s="13"/>
       <c r="N9" s="3">
         <f t="shared" si="0"/>
@@ -2816,12 +2886,15 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="B10" s="18">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="E10" s="4"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C10" s="42">
+        <v>0.125</v>
+      </c>
+      <c r="E10" s="1"/>
       <c r="F10" s="12"/>
       <c r="G10" s="1"/>
       <c r="H10" s="12"/>
@@ -2837,15 +2910,17 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="B11" s="18">
-        <v>8.3333333333333329E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="12"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="12"/>
+      <c r="H11" s="12">
+        <v>0.125</v>
+      </c>
       <c r="I11" s="1"/>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
@@ -2853,19 +2928,21 @@
       <c r="M11" s="13"/>
       <c r="N11" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" s="18">
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="12"/>
-      <c r="G12" s="1"/>
+      <c r="G12" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="H12" s="12"/>
       <c r="I12" s="1"/>
       <c r="J12" s="12"/>
@@ -2874,19 +2951,21 @@
       <c r="M12" s="13"/>
       <c r="N12" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+        <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" s="18">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="E13" s="1"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E13" s="4"/>
       <c r="F13" s="12"/>
-      <c r="G13" s="1"/>
+      <c r="G13" s="4">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="H13" s="12"/>
       <c r="I13" s="1"/>
       <c r="J13" s="12"/>
@@ -2895,19 +2974,21 @@
       <c r="M13" s="13"/>
       <c r="N13" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B14" s="18">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="E14" s="4"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E14" s="1"/>
       <c r="F14" s="12"/>
-      <c r="G14" s="1"/>
+      <c r="G14" s="4">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="H14" s="12"/>
       <c r="I14" s="1"/>
       <c r="J14" s="12"/>
@@ -2916,21 +2997,19 @@
       <c r="M14" s="13"/>
       <c r="N14" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="38" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" s="18">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="12"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E15" s="4"/>
       <c r="F15" s="12"/>
-      <c r="G15" s="16"/>
+      <c r="G15" s="1"/>
       <c r="H15" s="12"/>
       <c r="I15" s="1"/>
       <c r="J15" s="12"/>
@@ -2938,22 +3017,22 @@
       <c r="L15" s="1"/>
       <c r="M15" s="13"/>
       <c r="N15" s="3">
-        <f t="shared" ref="N15:N31" si="1">SUM(C15:M15)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="38" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B16" s="18">
-        <v>0.20833333333333334</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="12"/>
-      <c r="E16" s="1"/>
+      <c r="E16" s="4"/>
       <c r="F16" s="12"/>
-      <c r="G16" s="4"/>
+      <c r="G16" s="16"/>
       <c r="H16" s="12"/>
       <c r="I16" s="1"/>
       <c r="J16" s="12"/>
@@ -2961,25 +3040,27 @@
       <c r="L16" s="1"/>
       <c r="M16" s="13"/>
       <c r="N16" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="N16:N33" si="1">SUM(C16:M16)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="4"/>
+      <c r="A17" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="18">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="12"/>
-      <c r="E17" s="4"/>
+      <c r="E17" s="1"/>
       <c r="F17" s="12"/>
       <c r="G17" s="4"/>
       <c r="H17" s="12"/>
-      <c r="I17" s="4"/>
+      <c r="I17" s="1"/>
       <c r="J17" s="12"/>
       <c r="K17" s="12"/>
-      <c r="L17" s="4"/>
+      <c r="L17" s="1"/>
       <c r="M17" s="13"/>
       <c r="N17" s="3">
         <f t="shared" si="1"/>
@@ -2987,16 +3068,12 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="18">
-        <v>2.0833333333333332E-2</v>
-      </c>
+      <c r="A18" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="18"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="12">
-        <v>2.0833333333333332E-2</v>
-      </c>
+      <c r="D18" s="12"/>
       <c r="E18" s="4"/>
       <c r="F18" s="12"/>
       <c r="G18" s="4"/>
@@ -3008,21 +3085,21 @@
       <c r="M18" s="13"/>
       <c r="N18" s="3">
         <f t="shared" si="1"/>
-        <v>2.0833333333333332E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="37" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B19" s="18">
-        <v>8.3333333333333329E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="C19" s="4"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="4">
-        <v>6.25E-2</v>
-      </c>
+      <c r="D19" s="12">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E19" s="4"/>
       <c r="F19" s="12"/>
       <c r="G19" s="4"/>
       <c r="H19" s="12"/>
@@ -3033,20 +3110,20 @@
       <c r="M19" s="13"/>
       <c r="N19" s="3">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="37" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B20" s="18">
-        <v>2.0833333333333332E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="12"/>
       <c r="E20" s="4">
-        <v>2.0833333333333332E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="F20" s="12"/>
       <c r="G20" s="4"/>
@@ -3058,20 +3135,20 @@
       <c r="M20" s="13"/>
       <c r="N20" s="3">
         <f t="shared" si="1"/>
-        <v>2.0833333333333332E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="38" t="s">
-        <v>38</v>
+      <c r="A21" s="37" t="s">
+        <v>39</v>
       </c>
       <c r="B21" s="18">
-        <v>8.3333333333333329E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="12"/>
       <c r="E21" s="4">
-        <v>8.3333333333333329E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="F21" s="12"/>
       <c r="G21" s="4"/>
@@ -3083,12 +3160,12 @@
       <c r="M21" s="13"/>
       <c r="N21" s="3">
         <f t="shared" si="1"/>
-        <v>8.3333333333333329E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="37" t="s">
-        <v>60</v>
+      <c r="A22" s="38" t="s">
+        <v>38</v>
       </c>
       <c r="B22" s="18">
         <v>8.3333333333333329E-2</v>
@@ -3113,12 +3190,16 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="37" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" s="18"/>
+        <v>60</v>
+      </c>
+      <c r="B23" s="18">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="C23" s="4"/>
       <c r="D23" s="12"/>
-      <c r="E23" s="4"/>
+      <c r="E23" s="4">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="F23" s="12"/>
       <c r="G23" s="4"/>
       <c r="H23" s="12"/>
@@ -3127,17 +3208,22 @@
       <c r="K23" s="12"/>
       <c r="L23" s="4"/>
       <c r="M23" s="13"/>
-      <c r="N23" s="3"/>
+      <c r="N23" s="3">
+        <f t="shared" si="1"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B24" s="18"/>
       <c r="C24" s="4"/>
       <c r="D24" s="12"/>
       <c r="E24" s="4"/>
-      <c r="F24" s="12"/>
+      <c r="F24" s="12">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="G24" s="4"/>
       <c r="H24" s="12"/>
       <c r="I24" s="4"/>
@@ -3148,14 +3234,16 @@
       <c r="N24" s="3"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="35" t="s">
-        <v>22</v>
+      <c r="A25" s="37" t="s">
+        <v>62</v>
       </c>
       <c r="B25" s="18"/>
       <c r="C25" s="4"/>
       <c r="D25" s="12"/>
       <c r="E25" s="4"/>
-      <c r="F25" s="12"/>
+      <c r="F25" s="12">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="G25" s="4"/>
       <c r="H25" s="12"/>
       <c r="I25" s="4"/>
@@ -3163,50 +3251,42 @@
       <c r="K25" s="12"/>
       <c r="L25" s="4"/>
       <c r="M25" s="13"/>
-      <c r="N25" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="N25" s="3"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" s="18">
-        <v>2.0833333333333332E-2</v>
-      </c>
+      <c r="A26" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="18"/>
       <c r="C26" s="4"/>
       <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
+      <c r="E26" s="4"/>
       <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="12">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="I26" s="4"/>
       <c r="J26" s="12"/>
       <c r="K26" s="12"/>
-      <c r="L26" s="12"/>
+      <c r="L26" s="4"/>
       <c r="M26" s="13"/>
-      <c r="N26" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="N26" s="3"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" s="18">
-        <v>2.0833333333333332E-2</v>
-      </c>
+      <c r="A27" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="18"/>
       <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
+      <c r="D27" s="12"/>
       <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
+      <c r="F27" s="12"/>
       <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
+      <c r="H27" s="12"/>
       <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
       <c r="L27" s="4"/>
       <c r="M27" s="13"/>
       <c r="N27" s="3">
@@ -3216,38 +3296,48 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="36" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="B28" s="18">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="I28" s="12">
+        <v>0.125</v>
+      </c>
+      <c r="J28" s="12">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="K28" s="12">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="L28" s="12"/>
       <c r="M28" s="13"/>
       <c r="N28" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="36" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="B29" s="18">
-        <v>0.125</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
+      <c r="F29" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
@@ -3257,327 +3347,473 @@
       <c r="M29" s="13"/>
       <c r="N29" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="36" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="B30" s="18">
-        <v>0.125</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
+      <c r="G30" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
-      <c r="M30" s="15"/>
+      <c r="M30" s="13"/>
       <c r="N30" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="36" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B31" s="18">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="21"/>
-      <c r="K31" s="21"/>
-      <c r="L31" s="6"/>
-      <c r="M31" s="22"/>
+        <v>0.125</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="M31" s="13"/>
       <c r="N31" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="36" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="B32" s="18">
         <v>0.125</v>
       </c>
+      <c r="C32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="L32" s="4"/>
+      <c r="M32" s="15"/>
       <c r="N32" s="3">
-        <f t="shared" ref="N32:N42" si="2">SUM(C32:M32)</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.125</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="36" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="B33" s="18">
-        <v>8.3333333333333329E-2</v>
-      </c>
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C33" s="24"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="L33" s="4"/>
+      <c r="M33" s="13"/>
       <c r="N33" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B34" s="18">
-        <v>0.16666666666666666</v>
-      </c>
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G34" s="42">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="M34" s="51"/>
       <c r="N34" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" ref="N34:N45" si="2">SUM(C34:M34)</f>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="B35" s="18"/>
+      <c r="A35" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="18">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="J35" s="42">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="M35" s="51"/>
       <c r="N35" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="36" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="B36" s="18">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="D36" s="42">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="E36" s="42">
-        <v>4.1666666666666664E-2</v>
-      </c>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="J36" s="42">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="K36" s="42">
+        <v>0.125</v>
+      </c>
+      <c r="M36" s="51"/>
       <c r="N36" s="3">
         <f t="shared" si="2"/>
-        <v>6.25E-2</v>
+        <v>0.20833333333333331</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="36" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="B37" s="18">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="N37" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="J37" s="42">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="M37" s="51"/>
+      <c r="N37" s="3"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="B38" s="18">
-        <v>8.3333333333333329E-2</v>
-      </c>
+      <c r="A38" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38" s="18"/>
+      <c r="M38" s="51"/>
       <c r="N38" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="B39" s="18"/>
+      <c r="A39" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B39" s="18">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D39" s="42">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E39" s="42">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F39" s="42">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="G39" s="42">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="H39" s="42">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="I39" s="42">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="K39" s="42">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="M39" s="51"/>
       <c r="N39" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.3125</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="36" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B40" s="18">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="C40" s="42">
-        <v>6.25E-2</v>
-      </c>
-      <c r="D40" s="42">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="E40" s="42">
-        <v>0.10416666666666667</v>
-      </c>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="L40" s="42">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="M40" s="51"/>
       <c r="N40" s="3">
         <f t="shared" si="2"/>
-        <v>0.20833333333333331</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="36" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B41" s="18">
-        <v>0.33333333333333331</v>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="K41" s="42">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="M41" s="53">
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="N41" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="B42" s="18">
-        <v>8.3333333333333329E-2</v>
-      </c>
+      <c r="A42" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B42" s="18"/>
+      <c r="M42" s="51"/>
       <c r="N42" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="31"/>
+      <c r="A43" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B43" s="18">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C43" s="42">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D43" s="42">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E43" s="42">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="F43" s="42">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="G43" s="42">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="H43" s="42">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="I43" s="42">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="J43" s="42">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="K43" s="42">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="L43" s="42">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="M43" s="53">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="N43" s="3">
+        <f t="shared" si="2"/>
+        <v>0.58333333333333326</v>
+      </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="31"/>
-    </row>
-    <row r="45" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="32"/>
-      <c r="B45" s="3">
-        <f>SUM(B15:B31)</f>
-        <v>0.97916666666666674</v>
-      </c>
-      <c r="C45" s="3">
-        <f>SUM(C15:C31)</f>
+      <c r="A44" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="B44" s="18">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M44" s="53">
+        <v>0.125</v>
+      </c>
+      <c r="N44" s="3">
+        <f t="shared" si="2"/>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="B45" s="18">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="M45" s="53">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="N45" s="3">
+        <f t="shared" si="2"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" s="46"/>
+      <c r="B46" s="48"/>
+      <c r="M46" s="51"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" s="46"/>
+      <c r="B47" s="48"/>
+      <c r="M47" s="51"/>
+    </row>
+    <row r="48" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="47"/>
+      <c r="B48" s="49">
+        <f>SUM(B16:B33)</f>
+        <v>0.91666666666666674</v>
+      </c>
+      <c r="C48" s="50">
+        <f>SUM(C16:C33)</f>
         <v>0</v>
       </c>
-      <c r="D45" s="3">
-        <f>SUM(D15:D31)</f>
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="E45" s="3">
-        <f t="shared" ref="E45:M45" si="3">SUM(E2:E31)</f>
+      <c r="D48" s="50">
+        <f>SUM(D16:D33)</f>
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E48" s="50">
+        <f t="shared" ref="E48:M48" si="3">SUM(E2:E33)</f>
         <v>0.29166666666666663</v>
       </c>
-      <c r="F45" s="3">
+      <c r="F48" s="50">
+        <f t="shared" si="3"/>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="G48" s="50">
+        <f t="shared" si="3"/>
+        <v>0.12499999999999999</v>
+      </c>
+      <c r="H48" s="50">
+        <f t="shared" si="3"/>
+        <v>0.22916666666666669</v>
+      </c>
+      <c r="I48" s="50">
+        <f t="shared" si="3"/>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="J48" s="50">
+        <f t="shared" si="3"/>
+        <v>0.10416666666666666</v>
+      </c>
+      <c r="K48" s="50">
+        <f t="shared" si="3"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="L48" s="50">
+        <f t="shared" si="3"/>
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="M48" s="52">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G45" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H45" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I45" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J45" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K45" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L45" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M45" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="M46" s="3">
-        <f>SUM(C45:M45)</f>
-        <v>0.31249999999999994</v>
-      </c>
-      <c r="N46" s="3">
-        <f>SUM(N2:N42)</f>
-        <v>0.54166666666666663</v>
+    </row>
+    <row r="49" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M49" s="3">
+        <f>SUM(C48:M48)</f>
+        <v>1.2916666666666665</v>
+      </c>
+      <c r="N49" s="3">
+        <f>SUM(N2:N45)</f>
+        <v>2.6249999999999996</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:M2 F27:F29 H27:I29 E3:E21 G3:G21 I3:I21 L3:L21 C25:C31 G25:G31 I25:I26 I30:I31 E25:E31 L25:L31 C15:C21">
-    <cfRule type="cellIs" dxfId="18" priority="17" operator="greaterThan">
+  <conditionalFormatting sqref="E2:M2 F29:F31 H29:I31 E3:E22 G3:G22 I3:I22 L3:L22 C27:C33 G27:G33 I27:I28 I32:I33 E27:E33 L27:L33 C16:C22">
+    <cfRule type="cellIs" dxfId="20" priority="17" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:M2 E4:M12 C15:M21 C25:M29 C31:M31 C30 E30:M30 E14:M14">
-    <cfRule type="cellIs" dxfId="17" priority="16" operator="greaterThan">
+  <conditionalFormatting sqref="E2:M2 E4:M13 C16:M22 C27:M31 C33:M33 C32 E32:M32 E15:M15">
+    <cfRule type="cellIs" dxfId="19" priority="16" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L22:L24 I22:I24 G22:G24 E22:E24 C22:C24">
-    <cfRule type="cellIs" dxfId="16" priority="15" operator="greaterThan">
+  <conditionalFormatting sqref="L23:L26 I23:I26 G23:G26 E23:E26 C23:C26">
+    <cfRule type="cellIs" dxfId="18" priority="15" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C22:M24">
-    <cfRule type="cellIs" dxfId="15" priority="14" operator="greaterThan">
+  <conditionalFormatting sqref="C23:M26">
+    <cfRule type="cellIs" dxfId="17" priority="14" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J30:K30 F30 H30 M30">
-    <cfRule type="cellIs" dxfId="14" priority="13" operator="greaterThan">
+  <conditionalFormatting sqref="J32:K32 F32 H32 M32">
+    <cfRule type="cellIs" dxfId="16" priority="13" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D27:D29 G27:G29 J27:K29">
-    <cfRule type="cellIs" dxfId="13" priority="12" operator="greaterThan">
+  <conditionalFormatting sqref="D29:D31 G29:G31 J29:K31">
+    <cfRule type="cellIs" dxfId="15" priority="12" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C31:M31 C30 E30:M30 C15:M29 E2:M14">
-    <cfRule type="cellIs" dxfId="12" priority="9" operator="greaterThan">
+  <conditionalFormatting sqref="C33:M33 C32 E32:M32 C16:M31 E2:M15">
+    <cfRule type="cellIs" dxfId="14" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="11" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N15:N42">
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
-      <formula>$B15</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
-      <formula>$B15</formula>
+  <conditionalFormatting sqref="N16:N45">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="greaterThan">
+      <formula>$B16</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
+      <formula>$B16</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B45">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="greaterThan">
+  <conditionalFormatting sqref="B48">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="greaterThan">
       <formula>3.66666666666667</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>3.66666666666667</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C45:M45">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="greaterThan">
+  <conditionalFormatting sqref="C48:M48">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="greaterThan">
       <formula>0.333333333333333</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3630,7 +3866,30 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>N7:N14</xm:sqref>
+          <xm:sqref>N7:N8</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="59" operator="greaterThan" id="{BBEE44DB-A769-48ED-A8A4-03618C265174}">
+            <xm:f>Feuil1!$B6</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="9" tint="0.59996337778862885"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="60" operator="equal" id="{C0ECEFC0-4666-49C4-91D6-321A1BFD727B}">
+            <xm:f>Feuil1!$B6</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="6" tint="0.59996337778862885"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>N9:N15</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>